<commit_message>
test drift into original data
</commit_message>
<xml_diff>
--- a/final_ood_lapras.xlsx
+++ b/final_ood_lapras.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.48359375</v>
+        <v>0.865625</v>
       </c>
       <c r="C2" t="n">
-        <v>0.02335924435582196</v>
+        <v>0.05036487956651937</v>
       </c>
     </row>
     <row r="3">
@@ -461,10 +461,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.58359375</v>
+        <v>0.91171875</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05438532588736598</v>
+        <v>0.02981060004427956</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.86015625</v>
+        <v>0.8609375</v>
       </c>
       <c r="C4" t="n">
-        <v>0.04670542243010976</v>
+        <v>0.0488890245223813</v>
       </c>
     </row>
     <row r="5">
@@ -483,10 +483,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.8875</v>
+        <v>0.50078125</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07995512657500456</v>
+        <v>0.04631171979774666</v>
       </c>
     </row>
     <row r="6">
@@ -494,10 +494,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.84140625</v>
+        <v>0.91953125</v>
       </c>
       <c r="C6" t="n">
-        <v>0.08851255648917841</v>
+        <v>0.07430504851202911</v>
       </c>
     </row>
     <row r="7">
@@ -505,10 +505,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5984375</v>
+        <v>0.86796875</v>
       </c>
       <c r="C7" t="n">
-        <v>0.07499186153760286</v>
+        <v>0.02548360379734389</v>
       </c>
     </row>
     <row r="8">
@@ -516,10 +516,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.78828125</v>
+        <v>0.7953125</v>
       </c>
       <c r="C8" t="n">
-        <v>0.07903377689712798</v>
+        <v>0.03702498628460246</v>
       </c>
     </row>
     <row r="9">
@@ -527,10 +527,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.66015625</v>
+        <v>0.8</v>
       </c>
       <c r="C9" t="n">
-        <v>0.08999647345521379</v>
+        <v>0.05796011559684815</v>
       </c>
     </row>
     <row r="10">
@@ -538,10 +538,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.96640625</v>
+        <v>0.95859375</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02217979619777873</v>
+        <v>0.01858652695839113</v>
       </c>
     </row>
     <row r="11">
@@ -549,10 +549,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.54140625</v>
+        <v>0.853125</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0832901906551726</v>
+        <v>0.067775407482176</v>
       </c>
     </row>
     <row r="12">
@@ -560,10 +560,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.4437654613049464</v>
+        <v>0.8636114137295191</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03481862921325921</v>
+        <v>0.0517951208072918</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +571,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.545300820285353</v>
+        <v>0.9110256386483482</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0914016193680357</v>
+        <v>0.03030858880563073</v>
       </c>
     </row>
     <row r="14">
@@ -582,10 +582,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.8578398247430734</v>
+        <v>0.8582828815892848</v>
       </c>
       <c r="C14" t="n">
-        <v>0.04821188574262342</v>
+        <v>0.05177958285980839</v>
       </c>
     </row>
     <row r="15">
@@ -593,10 +593,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8851801621745971</v>
+        <v>0.4850990583433807</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0825056703533834</v>
+        <v>0.03702907266559296</v>
       </c>
     </row>
     <row r="16">
@@ -604,10 +604,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.8223808028758519</v>
+        <v>0.9185068986806142</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1186395578679433</v>
+        <v>0.07543230980102132</v>
       </c>
     </row>
     <row r="17">
@@ -615,10 +615,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5577213654494683</v>
+        <v>0.8656635937100488</v>
       </c>
       <c r="C17" t="n">
-        <v>0.09726491516147848</v>
+        <v>0.02748353941379713</v>
       </c>
     </row>
     <row r="18">
@@ -626,10 +626,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.7809473994724301</v>
+        <v>0.7807092927776933</v>
       </c>
       <c r="C18" t="n">
-        <v>0.08461696668921222</v>
+        <v>0.04632330621588953</v>
       </c>
     </row>
     <row r="19">
@@ -637,10 +637,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.6218493503981242</v>
+        <v>0.7752314982174235</v>
       </c>
       <c r="C19" t="n">
-        <v>0.1168062037608873</v>
+        <v>0.08767573598631108</v>
       </c>
     </row>
     <row r="20">
@@ -648,10 +648,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9662073127486972</v>
+        <v>0.9583769564759038</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02254374849569267</v>
+        <v>0.01897274130644477</v>
       </c>
     </row>
     <row r="21">
@@ -659,10 +659,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5138071992584632</v>
+        <v>0.8505828951995115</v>
       </c>
       <c r="C21" t="n">
-        <v>0.1007392482368634</v>
+        <v>0.06919544220630627</v>
       </c>
     </row>
     <row r="22">
@@ -670,10 +670,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.50653076171875</v>
+        <v>0.94879150390625</v>
       </c>
       <c r="C22" t="n">
-        <v>0.03120027400532249</v>
+        <v>0.03869328532308846</v>
       </c>
     </row>
     <row r="23">
@@ -681,10 +681,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.61748046875</v>
+        <v>0.9736083984375</v>
       </c>
       <c r="C23" t="n">
-        <v>0.07355619537380011</v>
+        <v>0.02417946367052349</v>
       </c>
     </row>
     <row r="24">
@@ -692,10 +692,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.9482421875</v>
+        <v>0.93121337890625</v>
       </c>
       <c r="C24" t="n">
-        <v>0.02229199103241224</v>
+        <v>0.0260944530826347</v>
       </c>
     </row>
     <row r="25">
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.94569091796875</v>
+        <v>0.50902099609375</v>
       </c>
       <c r="C25" t="n">
-        <v>0.05747054755514734</v>
+        <v>0.0656675246379526</v>
       </c>
     </row>
     <row r="26">
@@ -714,10 +714,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.97191162109375</v>
+        <v>0.986767578125</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01485858978539397</v>
+        <v>0.02465875908253204</v>
       </c>
     </row>
     <row r="27">
@@ -725,10 +725,10 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.67701416015625</v>
+        <v>0.95079345703125</v>
       </c>
       <c r="C27" t="n">
-        <v>0.05131886461119931</v>
+        <v>0.04838541984215908</v>
       </c>
     </row>
     <row r="28">
@@ -736,10 +736,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8916748046875</v>
+        <v>0.951025390625</v>
       </c>
       <c r="C28" t="n">
-        <v>0.07269655975796875</v>
+        <v>0.04990334705755102</v>
       </c>
     </row>
     <row r="29">
@@ -747,10 +747,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.7451416015625</v>
+        <v>0.9190185546875</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1018909249993786</v>
+        <v>0.035887642151469</v>
       </c>
     </row>
     <row r="30">
@@ -758,10 +758,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.99129638671875</v>
+        <v>0.99442138671875</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01170485626575681</v>
+        <v>0.002847563146840495</v>
       </c>
     </row>
     <row r="31">
@@ -769,10 +769,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.52017822265625</v>
+        <v>0.95325927734375</v>
       </c>
       <c r="C31" t="n">
-        <v>0.08253417116575971</v>
+        <v>0.03112659885329115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>